<commit_message>
Popup on user hover implemented
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,13 +800,15 @@
       <c r="B16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D16" s="5">
         <v>10</v>
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>38</v>
       </c>
@@ -818,7 +820,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>39</v>
       </c>
@@ -830,7 +832,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>40</v>
       </c>
@@ -842,7 +844,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>41</v>
       </c>
@@ -854,7 +856,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
@@ -866,11 +868,13 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" s="5">
         <v>10</v>
       </c>
@@ -912,7 +916,9 @@
       <c r="B26" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D26" s="5">
         <v>10</v>
       </c>
@@ -922,7 +928,9 @@
       <c r="B27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D27" s="5">
         <v>10</v>
       </c>
@@ -952,7 +960,9 @@
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D30" s="5">
         <v>10</v>
       </c>
@@ -1024,7 +1034,9 @@
       <c r="B37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="D37" s="7">
         <v>5</v>
       </c>

</xml_diff>